<commit_message>
Update them giao dien quy trinh
</commit_message>
<xml_diff>
--- a/quytrinh.xlsx
+++ b/quytrinh.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Other computers\My PC HOME\code\"/>
@@ -12,15 +12,54 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6610"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="QuyTrinh" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>Tên quy trình</t>
+  </si>
+  <si>
+    <t>tesst</t>
+  </si>
+  <si>
+    <t>Bí danh quy trình</t>
+  </si>
+  <si>
+    <t>t1</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Tên Form</t>
+  </si>
+  <si>
+    <t>Mã Action</t>
+  </si>
+  <si>
+    <t>Thời gian</t>
+  </si>
+  <si>
+    <t>Nhóm người dùng</t>
+  </si>
+  <si>
+    <t>Theen moiu</t>
+  </si>
+  <si>
+    <t>Thêm mới</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>chuyen vien</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -31,7 +70,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -62,7 +100,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -85,44 +123,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -149,15 +187,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -184,7 +221,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -196,153 +232,235 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update cau hinh quy trinh
</commit_message>
<xml_diff>
--- a/quytrinh.xlsx
+++ b/quytrinh.xlsx
@@ -1,81 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Other computers\My PC HOME\code\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6610"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="QuyTrinh" sheetId="1" r:id="rId1"/>
+    <sheet name="QuyTrinh" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Tên quy trình</t>
-  </si>
-  <si>
-    <t>tesst</t>
-  </si>
-  <si>
-    <t>Bí danh quy trình</t>
-  </si>
-  <si>
-    <t>t1</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Tên Form</t>
-  </si>
-  <si>
-    <t>Mã Action</t>
-  </si>
-  <si>
-    <t>Thời gian</t>
-  </si>
-  <si>
-    <t>Nhóm người dùng</t>
-  </si>
-  <si>
-    <t>Theen moiu</t>
-  </si>
-  <si>
-    <t>Thêm mới</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>chuyen vien</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -94,21 +47,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -396,68 +408,124 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.90625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Tên quy trình</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Bí danh</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Tên Form</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Mã Action</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Thời gian</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Nhóm người dùng</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Quy trình xử lý hồ sơ một cửa</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>QT Test</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>1</v>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Thêm mới</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Thêm mới</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>chuyên viên</t>
+        </is>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Quy trình xử lý hồ sơ một cửa</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>QT Test</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chuyển phòng chuyên môn </t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Chuyển xử lý</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>lãnh đạo</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chinh giao dien excel
</commit_message>
<xml_diff>
--- a/quytrinh.xlsx
+++ b/quytrinh.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="QuyTrinh" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="LuanChuyen" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,13 +18,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +50,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,131 +429,209 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Tên quy trình</t>
+          <t>Tên quy trình:</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Xử lý hồ sơ một cửa</t>
+          <t>Quy trình 1 cửa</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Bí danh quy trình</t>
+          <t>Bí danh:</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>QT- 1c</t>
+          <t>QT 1C</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Gắn vào TTHC:</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>H13.111111233</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>TTHC</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
           <t>Tên quy trình</t>
         </is>
       </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>Tên Form</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>Mã Action</t>
+        </is>
+      </c>
+      <c r="F5" s="1" t="inlineStr">
+        <is>
+          <t>Thời gian</t>
+        </is>
+      </c>
+      <c r="G5" s="1" t="inlineStr">
+        <is>
+          <t>Nhóm người dùng</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>H13.111111233</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Quy trình 1 cửa</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Thêm mới</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Thêm mới</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>CV</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Tên quy trình:</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Quy trình 1 cửa</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Bí danh:</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>QT 1C</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Gắn vào TTHC:</t>
+        </is>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Bí danh</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Tên Form</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Mã Action</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Thời gian</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Nhóm người dùng</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Xử lý hồ sơ một cửa</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>QT- 1c</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="inlineStr">
+          <t>H13.111111233</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Từ Form</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>Đến Form</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>Đến Form 2</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>Đến Form 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
         <is>
           <t>Thêm mới</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>Thêm mới</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Một cửa</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Xử lý hồ sơ một cửa</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>QT- 1c</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Chuyển xử lý</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Chuyển xử lý</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Chuyên viên</t>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Thêm mới</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Thêm mới</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
cau hinh luan chuyen
</commit_message>
<xml_diff>
--- a/quytrinh.xlsx
+++ b/quytrinh.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,7 +434,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Quy trình test</t>
+          <t>Quy trình xử lý hồ sơ 1 cửa</t>
         </is>
       </c>
     </row>
@@ -446,7 +446,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>T1</t>
+          <t>QT 1C</t>
         </is>
       </c>
     </row>
@@ -456,7 +456,11 @@
           <t>Gắn vào TTHC:</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>H13-12345-1</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -501,15 +505,19 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>H13-12345-1</t>
+        </is>
+      </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Quy trình test</t>
+          <t>Quy trình xử lý hồ sơ 1 cửa</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>T1</t>
+          <t>QT 1C</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -519,22 +527,190 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
+          <t xml:space="preserve">Tiếp nhận hồ sơ </t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
           <t>Thêm mới</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Thêm mới</t>
-        </is>
-      </c>
       <c r="G6" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Một cửa</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>H13-12345-1</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Quy trình xử lý hồ sơ 1 cửa</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>QT 1C</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Thẩm tra tại đơn vị</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Chuyển xử lý</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Chuyên viên</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>H13-12345-1</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Quy trình xử lý hồ sơ 1 cửa</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>QT 1C</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Chuyên viên</t>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Trình lãnh đạo phê duyệt dự thảo</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Trình phê duyệt</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Lãnh đạo đơn vị</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>H13-12345-1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Quy trình xử lý hồ sơ 1 cửa</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>QT 1C</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Đóng dấu văn bản</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Chuyển ban hành</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Lãnh đạo phòng</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>H13-12345-1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Quy trình xử lý hồ sơ 1 cửa</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>QT 1C</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Chuyển trả kết quả</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Chuyển trả kết quả</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Một cửa</t>
         </is>
       </c>
     </row>
@@ -549,7 +725,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -565,7 +741,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Quy trình test</t>
+          <t>Quy trình xử lý hồ sơ 1 cửa</t>
         </is>
       </c>
     </row>
@@ -577,7 +753,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>T1</t>
+          <t>QT 1C</t>
         </is>
       </c>
     </row>
@@ -587,7 +763,11 @@
           <t>Gắn vào TTHC:</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>H13-12345-1</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -614,24 +794,70 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Thêm mới</t>
+          <t xml:space="preserve">Tiếp nhận hồ sơ </t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Thêm mới</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Thêm mới</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Thêm mới</t>
-        </is>
-      </c>
+          <t>Thẩm tra tại đơn vị</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Thẩm tra tại đơn vị</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Trình lãnh đạo phê duyệt dự thảo</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Chuyển trả kết quả</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Trình lãnh đạo phê duyệt dự thảo</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Đóng dấu văn bản</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Thẩm tra tại đơn vị</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Đóng dấu văn bản</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Chuyển trả kết quả</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Trình lãnh đạo phê duyệt dự thảo</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>